<commit_message>
added logic of image creation of all schedules and machine req
</commit_message>
<xml_diff>
--- a/input_data/Requirements (1).xlsx
+++ b/input_data/Requirements (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="11496" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="InfeasibleOutput (2)" sheetId="5" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:CS9"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="BK8" sqref="BK8"/>
+    <sheetView topLeftCell="AT1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="BT1" sqref="BT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1423,7 +1423,7 @@
   <dimension ref="A2:BU10"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4098,8 +4098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:CS9"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="AT15" sqref="AT15"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5059,7 +5059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>